<commit_message>
Add Day 40 Project: Flight ClubF
</commit_message>
<xml_diff>
--- a/day-039-project-flight-deal-finder/template_sheet/Flight Deals.xlsx
+++ b/day-039-project-flight-deal-finder/template_sheet/Flight Deals.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="prices" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="users" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>City</t>
   </si>
@@ -74,13 +75,46 @@
   </si>
   <si>
     <t>CPT</t>
+  </si>
+  <si>
+    <t>Bali</t>
+  </si>
+  <si>
+    <t>DPS</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Name1</t>
+  </si>
+  <si>
+    <t>LastName1</t>
+  </si>
+  <si>
+    <t>email1@gmail.com</t>
+  </si>
+  <si>
+    <t>Name2</t>
+  </si>
+  <si>
+    <t>LastName2</t>
+  </si>
+  <si>
+    <t>email2@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -95,6 +129,17 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -111,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -130,6 +175,13 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -139,6 +191,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -366,7 +422,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="4">
-        <v>54.0</v>
+        <v>76.0</v>
       </c>
       <c r="D2" s="2"/>
     </row>
@@ -465,6 +521,91 @@
         <v>378.0</v>
       </c>
       <c r="D10" s="2"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="6">
+        <v>501.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="3" max="3" width="20.13"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>